<commit_message>
Fix Excel import tests
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/tube-checkin.xlsx
+++ b/tests/ExcelImport/workbooks/tube-checkin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D9934E-4559-5C4D-AEAF-814347EB6874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8713C5C-59F1-174D-8C81-44B875C56193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{D641F29D-EB73-5746-B974-A2176733CB0B}"/>
   </bookViews>
@@ -50,27 +50,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>TEST0001</t>
-  </si>
-  <si>
-    <t>TEST0002</t>
-  </si>
-  <si>
-    <t>TEST0003</t>
-  </si>
-  <si>
-    <t>TEST0004</t>
-  </si>
-  <si>
-    <t>TEST0005</t>
-  </si>
-  <si>
-    <t>TEST0006</t>
-  </si>
-  <si>
-    <t>TEST0007</t>
-  </si>
-  <si>
     <t>Accepted</t>
   </si>
   <si>
@@ -87,6 +66,27 @@
   </si>
   <si>
     <t>jok</t>
+  </si>
+  <si>
+    <t>TestCheckin0001</t>
+  </si>
+  <si>
+    <t>TestCheckin0002</t>
+  </si>
+  <si>
+    <t>TestCheckin0003</t>
+  </si>
+  <si>
+    <t>TestCheckin0004</t>
+  </si>
+  <si>
+    <t>TestCheckin0005</t>
+  </si>
+  <si>
+    <t>TestCheckin0006</t>
+  </si>
+  <si>
+    <t>TestCheckin0007</t>
   </si>
 </sst>
 </file>
@@ -447,11 +447,12 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
@@ -476,115 +477,115 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests cover Excel import with empty rows
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/tube-checkin.xlsx
+++ b/tests/ExcelImport/workbooks/tube-checkin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8713C5C-59F1-174D-8C81-44B875C56193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3924CE6D-5721-9747-A1AB-5845716D57B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{D641F29D-EB73-5746-B974-A2176733CB0B}"/>
   </bookViews>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966E636C-4996-8A44-87BF-81C75963A000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,32 +509,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -542,7 +525,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -551,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -559,13 +542,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -573,18 +559,32 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>